<commit_message>
added 3 comp excel, fixed towns
</commit_message>
<xml_diff>
--- a/2.xlsx
+++ b/2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hackathon2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775AC779-6741-4786-A7E2-69BBC400BE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38135AB5-D111-4E20-82D9-838EFC8575D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="866" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Основные параметры оценки" sheetId="1" r:id="rId1"/>
@@ -536,9 +536,6 @@
     <t>TELE2</t>
   </si>
   <si>
-    <t>Место проведения контроля: г. Екатеринбург</t>
-  </si>
-  <si>
     <t>Время проведения контроля:  с 12.01.2022 по 17.04.2022</t>
   </si>
   <si>
@@ -546,6 +543,9 @@
   </si>
   <si>
     <t>ПРОТОКОЛ КОНТРОЛЯ ПАРАМЕТРОВ КАЧЕСТВА УСЛУГ ПОДВИЖНОЙ РАДИОТЕЛЕФОННОЙ СВЯЗИ № 32 от «18» апреля 2022 г.</t>
+  </si>
+  <si>
+    <t>Место проведения контроля: г. Челябинск</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -729,6 +729,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -1151,7 +1157,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
@@ -1344,6 +1350,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1802,8 +1811,8 @@
   </sheetPr>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:F12"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1819,100 +1828,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="84" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="84"/>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="80" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
     </row>
     <row r="4" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="81" t="s">
+        <v>166</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="80"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="82" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="80"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
-    </row>
-    <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
-        <v>168</v>
-      </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -1923,54 +1932,54 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="78" t="s">
         <v>160</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="77" t="s">
-        <v>166</v>
-      </c>
-      <c r="B13" s="77"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
+      <c r="A13" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="78"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="77"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
+      <c r="A14" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="78"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="78"/>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
+      <c r="B16" s="79"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
     </row>
     <row r="17" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
@@ -2040,7 +2049,7 @@
       <c r="B20" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="C20" s="63">
+      <c r="C20" s="77">
         <v>6.7376288659793797</v>
       </c>
       <c r="D20" s="63">
@@ -3063,32 +3072,32 @@
       </c>
     </row>
     <row r="41" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="86"/>
-      <c r="K41" s="86"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="87"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="I41" s="87"/>
+      <c r="J41" s="87"/>
+      <c r="K41" s="87"/>
     </row>
     <row r="42" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="86"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="86"/>
-      <c r="F42" s="86"/>
-      <c r="G42" s="86"/>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="86"/>
-      <c r="K42" s="86"/>
+      <c r="A42" s="87"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="87"/>
+      <c r="E42" s="87"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="87"/>
     </row>
     <row r="43" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K43" s="37"/>
@@ -3439,32 +3448,32 @@
       </c>
     </row>
     <row r="64" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="87" t="s">
+      <c r="A64" s="88" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="88"/>
-      <c r="C64" s="88"/>
-      <c r="D64" s="88"/>
-      <c r="E64" s="88"/>
-      <c r="F64" s="88"/>
-      <c r="G64" s="88"/>
-      <c r="H64" s="88"/>
-      <c r="I64" s="88"/>
-      <c r="J64" s="88"/>
-      <c r="K64" s="88"/>
+      <c r="B64" s="89"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="89"/>
+      <c r="E64" s="89"/>
+      <c r="F64" s="89"/>
+      <c r="G64" s="89"/>
+      <c r="H64" s="89"/>
+      <c r="I64" s="89"/>
+      <c r="J64" s="89"/>
+      <c r="K64" s="89"/>
     </row>
     <row r="65" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="88"/>
-      <c r="B65" s="88"/>
-      <c r="C65" s="88"/>
-      <c r="D65" s="88"/>
-      <c r="E65" s="88"/>
-      <c r="F65" s="88"/>
-      <c r="G65" s="88"/>
-      <c r="H65" s="88"/>
-      <c r="I65" s="88"/>
-      <c r="J65" s="88"/>
-      <c r="K65" s="88"/>
+      <c r="A65" s="89"/>
+      <c r="B65" s="89"/>
+      <c r="C65" s="89"/>
+      <c r="D65" s="89"/>
+      <c r="E65" s="89"/>
+      <c r="F65" s="89"/>
+      <c r="G65" s="89"/>
+      <c r="H65" s="89"/>
+      <c r="I65" s="89"/>
+      <c r="J65" s="89"/>
+      <c r="K65" s="89"/>
     </row>
     <row r="67" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
@@ -4116,32 +4125,32 @@
     </row>
     <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="87" t="s">
+      <c r="A110" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="B110" s="88"/>
-      <c r="C110" s="88"/>
-      <c r="D110" s="88"/>
-      <c r="E110" s="88"/>
-      <c r="F110" s="88"/>
-      <c r="G110" s="88"/>
-      <c r="H110" s="88"/>
-      <c r="I110" s="88"/>
-      <c r="J110" s="88"/>
-      <c r="K110" s="88"/>
+      <c r="B110" s="89"/>
+      <c r="C110" s="89"/>
+      <c r="D110" s="89"/>
+      <c r="E110" s="89"/>
+      <c r="F110" s="89"/>
+      <c r="G110" s="89"/>
+      <c r="H110" s="89"/>
+      <c r="I110" s="89"/>
+      <c r="J110" s="89"/>
+      <c r="K110" s="89"/>
     </row>
     <row r="111" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="88"/>
-      <c r="B111" s="88"/>
-      <c r="C111" s="88"/>
-      <c r="D111" s="88"/>
-      <c r="E111" s="88"/>
-      <c r="F111" s="88"/>
-      <c r="G111" s="88"/>
-      <c r="H111" s="88"/>
-      <c r="I111" s="88"/>
-      <c r="J111" s="88"/>
-      <c r="K111" s="88"/>
+      <c r="A111" s="89"/>
+      <c r="B111" s="89"/>
+      <c r="C111" s="89"/>
+      <c r="D111" s="89"/>
+      <c r="E111" s="89"/>
+      <c r="F111" s="89"/>
+      <c r="G111" s="89"/>
+      <c r="H111" s="89"/>
+      <c r="I111" s="89"/>
+      <c r="J111" s="89"/>
+      <c r="K111" s="89"/>
     </row>
     <row r="112" spans="1:11" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="16"/>

</xml_diff>